<commit_message>
work deep 01 2023-04-04
</commit_message>
<xml_diff>
--- a/015 VBA Programming/07-10-getpivotdata-Complete.xlsx
+++ b/015 VBA Programming/07-10-getpivotdata-Complete.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web learning\015 VBA Programming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8F9AEA-E9CE-4AF0-A3BE-978A039EC44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F851BA4-EC7A-479B-B92C-F7F2DEECDAE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{FCA7320E-6CEF-47D9-9EBD-252F01CC21B9}"/>
   </bookViews>
@@ -3236,7 +3236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F32A9137-579B-4047-AC4A-AE1469FE03EE}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>

</xml_diff>